<commit_message>
Added hazards and hooked resources and hazards into new WorldMap_UI
</commit_message>
<xml_diff>
--- a/Data/WorldMap.xlsx
+++ b/Data/WorldMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lemon\Documents\GenomeEvolution\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A702842-E2EB-4DFC-AE3E-C1C50A8FDF17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900EB72A-8A7D-4C7F-B307-7A21C21E1CC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83D411EE-8B86-42BF-BF83-C6FED3856F58}"/>
+    <workbookView xWindow="3804" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{83D411EE-8B86-42BF-BF83-C6FED3856F58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C69E45E-AD30-4CD9-B51A-E67E15FBA8E9}">
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,27 +1166,23 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="6">
-        <v>-50</v>
-      </c>
-      <c r="F2" s="6">
-        <v>-30</v>
-      </c>
-      <c r="G2" s="7">
-        <v>30</v>
-      </c>
-      <c r="H2" s="7">
-        <v>40</v>
-      </c>
+      <c r="E2" s="7">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7">
+        <v>70</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -1194,61 +1190,79 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="7">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="F3" s="7">
-        <v>70</v>
+        <v>-30</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>100</v>
+      </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="E4" s="7">
-        <v>-70</v>
+        <v>-40</v>
       </c>
       <c r="F4" s="7">
-        <v>-50</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+        <v>-25</v>
+      </c>
+      <c r="G4" s="7">
+        <v>50</v>
+      </c>
+      <c r="H4" s="7">
+        <v>70</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>100</v>
+      </c>
+      <c r="K4" s="7">
+        <v>20</v>
+      </c>
+      <c r="L4" s="7">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="7">
@@ -1270,13 +1284,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="7">
@@ -1288,84 +1302,82 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7">
+        <v>-100</v>
+      </c>
+      <c r="J6" s="7">
         <v>0</v>
-      </c>
-      <c r="J6" s="7">
-        <v>100</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="7">
-        <v>30</v>
+        <v>-40</v>
       </c>
       <c r="F7" s="7">
-        <v>50</v>
+        <v>-25</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <v>100</v>
+      </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="7">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="F8" s="7">
-        <v>70</v>
-      </c>
-      <c r="G8" s="7">
-        <v>-10</v>
-      </c>
-      <c r="H8" s="7">
-        <v>10</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7">
+        <v>-30</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7">
         <v>-100</v>
       </c>
-      <c r="L8" s="7">
-        <v>-10</v>
-      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E9" s="7">
         <v>50</v>
@@ -1374,44 +1386,50 @@
         <v>70</v>
       </c>
       <c r="G9" s="7">
-        <v>-20</v>
+        <v>-10</v>
       </c>
       <c r="H9" s="7">
-        <v>20</v>
-      </c>
-      <c r="I9" s="7">
+        <v>10</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7">
+        <v>-100</v>
+      </c>
+      <c r="L9" s="7">
         <v>-10</v>
       </c>
-      <c r="J9" s="7">
-        <v>20</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E10" s="7">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="F10" s="7">
-        <v>-30</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="G10" s="7">
+        <v>-20</v>
+      </c>
+      <c r="H10" s="7">
+        <v>20</v>
+      </c>
       <c r="I10" s="7">
-        <v>-100</v>
+        <v>-10</v>
       </c>
       <c r="J10" s="7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
@@ -1446,57 +1464,53 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>-50</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>-30</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7">
-        <v>-100</v>
-      </c>
-      <c r="J12" s="7">
-        <v>0</v>
-      </c>
+      <c r="G12" s="7">
+        <v>30</v>
+      </c>
+      <c r="H12" s="7">
+        <v>40</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="7">
-        <v>-40</v>
+        <v>-70</v>
       </c>
       <c r="F13" s="7">
-        <v>-25</v>
+        <v>-50</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="7">
-        <v>0</v>
-      </c>
-      <c r="J13" s="7">
-        <v>100</v>
-      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
     </row>
@@ -1530,51 +1544,37 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D15" s="5"/>
       <c r="E15" s="7">
-        <v>-40</v>
+        <v>30</v>
       </c>
       <c r="F15" s="7">
-        <v>-25</v>
-      </c>
-      <c r="G15" s="7">
         <v>50</v>
       </c>
-      <c r="H15" s="7">
-        <v>70</v>
-      </c>
-      <c r="I15" s="7">
-        <v>0</v>
-      </c>
-      <c r="J15" s="7">
-        <v>100</v>
-      </c>
-      <c r="K15" s="7">
-        <v>20</v>
-      </c>
-      <c r="L15" s="7">
-        <v>100</v>
-      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="7">
@@ -2499,8 +2499,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:G31">
-    <sortCondition ref="A20:A31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
+    <sortCondition ref="A2:A17"/>
   </sortState>
   <mergeCells count="7">
     <mergeCell ref="B35:C35"/>

</xml_diff>

<commit_message>
Merged the new WorldMap and the CardTable together; some bugs are still present, but it at least runs
</commit_message>
<xml_diff>
--- a/Data/WorldMap.xlsx
+++ b/Data/WorldMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lemon\Documents\GenomeEvolution\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900EB72A-8A7D-4C7F-B307-7A21C21E1CC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA8B8C7-0196-48C4-855D-4F7CC4BA2129}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{83D411EE-8B86-42BF-BF83-C6FED3856F58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83D411EE-8B86-42BF-BF83-C6FED3856F58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
   <si>
     <t>Biome</t>
   </si>
@@ -42,15 +42,6 @@
     <t>steak</t>
   </si>
   <si>
-    <t>burger</t>
-  </si>
-  <si>
-    <t>chicken</t>
-  </si>
-  <si>
-    <t>bacon</t>
-  </si>
-  <si>
     <t>butter</t>
   </si>
   <si>
@@ -69,12 +60,6 @@
     <t>potato</t>
   </si>
   <si>
-    <t>spaghetti</t>
-  </si>
-  <si>
-    <t>pretzel</t>
-  </si>
-  <si>
     <t>vitamin</t>
   </si>
   <si>
@@ -150,15 +135,6 @@
     <t>Group</t>
   </si>
   <si>
-    <t>lipids</t>
-  </si>
-  <si>
-    <t>carbohydrates</t>
-  </si>
-  <si>
-    <t>proteins</t>
-  </si>
-  <si>
     <t>minerals</t>
   </si>
   <si>
@@ -196,6 +172,45 @@
   </si>
   <si>
     <t xml:space="preserve">Heavy Metals (mg/kg: 10, 67) </t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>candy_1</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>protein_shake</t>
+  </si>
+  <si>
+    <t>carbohydrates_1</t>
+  </si>
+  <si>
+    <t>carbohydrates_2</t>
+  </si>
+  <si>
+    <t>fats_1</t>
+  </si>
+  <si>
+    <t>fats_2</t>
+  </si>
+  <si>
+    <t>proteins_1</t>
+  </si>
+  <si>
+    <t>proteins_2</t>
   </si>
 </sst>
 </file>
@@ -417,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -479,6 +494,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,549 +1122,651 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C69E45E-AD30-4CD9-B51A-E67E15FBA8E9}">
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="7">
-        <v>50</v>
-      </c>
-      <c r="F2" s="7">
-        <v>70</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="C2" s="29">
+        <v>1</v>
+      </c>
+      <c r="D2" s="29">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="7">
+        <v>-50</v>
+      </c>
+      <c r="H2" s="7">
+        <v>-30</v>
+      </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K2" s="7">
+        <v>-100</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0</v>
+      </c>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="7">
+        <v>54</v>
+      </c>
+      <c r="C3" s="29">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7">
         <v>-50</v>
       </c>
-      <c r="F3" s="7">
+      <c r="H3" s="7">
         <v>-30</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7">
-        <v>0</v>
-      </c>
-      <c r="J3" s="7">
-        <v>100</v>
-      </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7">
+        <v>-100</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="29">
+        <v>1</v>
+      </c>
+      <c r="D4" s="29">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="7">
-        <v>-40</v>
-      </c>
-      <c r="F4" s="7">
-        <v>-25</v>
-      </c>
+      <c r="F4" s="5"/>
       <c r="G4" s="7">
+        <v>-70</v>
+      </c>
+      <c r="H4" s="7">
+        <v>-50</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0</v>
+      </c>
+      <c r="D5" s="29">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="7">
+        <v>30</v>
+      </c>
+      <c r="H5" s="7">
         <v>50</v>
       </c>
-      <c r="H4" s="7">
-        <v>70</v>
-      </c>
-      <c r="I4" s="7">
-        <v>0</v>
-      </c>
-      <c r="J4" s="7">
-        <v>100</v>
-      </c>
-      <c r="K4" s="7">
-        <v>20</v>
-      </c>
-      <c r="L4" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7">
-        <v>-50</v>
-      </c>
-      <c r="F5" s="7">
-        <v>-30</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7">
-        <v>-100</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="7">
-        <v>-50</v>
-      </c>
-      <c r="F6" s="7">
-        <v>-30</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7">
-        <v>-100</v>
-      </c>
-      <c r="J6" s="7">
-        <v>0</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C6" s="29">
+        <v>1</v>
+      </c>
+      <c r="D6" s="29">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="7">
+        <v>50</v>
+      </c>
+      <c r="H6" s="7">
+        <v>70</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7">
+        <v>57</v>
+      </c>
+      <c r="C7" s="29">
+        <v>0</v>
+      </c>
+      <c r="D7" s="29">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="7">
         <v>-40</v>
       </c>
-      <c r="F7" s="7">
+      <c r="H7" s="7">
         <v>-25</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7">
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
         <v>100</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="29">
+        <v>0</v>
+      </c>
+      <c r="D8" s="29">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="7">
+        <v>-40</v>
+      </c>
+      <c r="H8" s="7">
+        <v>-25</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
+        <v>100</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="29">
+        <v>1</v>
+      </c>
+      <c r="D9" s="29">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6">
+        <v>-50</v>
+      </c>
+      <c r="H9" s="6">
+        <v>-30</v>
+      </c>
+      <c r="I9" s="7">
+        <v>30</v>
+      </c>
+      <c r="J9" s="7">
+        <v>40</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="29">
+        <v>0</v>
+      </c>
+      <c r="D10" s="29">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="7">
+        <v>-40</v>
+      </c>
+      <c r="H10" s="7">
+        <v>-25</v>
+      </c>
+      <c r="I10" s="7">
+        <v>50</v>
+      </c>
+      <c r="J10" s="7">
+        <v>70</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10" s="7">
+        <v>100</v>
+      </c>
+      <c r="M10" s="7">
+        <v>20</v>
+      </c>
+      <c r="N10" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="29">
+        <v>0</v>
+      </c>
+      <c r="D11" s="29">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7">
-        <v>-50</v>
-      </c>
-      <c r="F8" s="7">
-        <v>-30</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7">
-        <v>-100</v>
-      </c>
-      <c r="J8" s="7">
-        <v>0</v>
-      </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="G11" s="7">
         <v>50</v>
       </c>
-      <c r="F9" s="7">
+      <c r="H11" s="7">
         <v>70</v>
       </c>
-      <c r="G9" s="7">
+      <c r="I11" s="7">
         <v>-10</v>
       </c>
-      <c r="H9" s="7">
+      <c r="J11" s="7">
         <v>10</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7">
-        <v>-100</v>
-      </c>
-      <c r="L9" s="7">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="7">
-        <v>50</v>
-      </c>
-      <c r="F10" s="7">
-        <v>70</v>
-      </c>
-      <c r="G10" s="7">
-        <v>-20</v>
-      </c>
-      <c r="H10" s="7">
-        <v>20</v>
-      </c>
-      <c r="I10" s="7">
-        <v>-10</v>
-      </c>
-      <c r="J10" s="7">
-        <v>20</v>
-      </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="7">
-        <v>-40</v>
-      </c>
-      <c r="F11" s="7">
-        <v>-25</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7">
-        <v>0</v>
-      </c>
-      <c r="J11" s="7">
-        <v>100</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="7">
+        <v>-100</v>
+      </c>
+      <c r="N11" s="7">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6">
-        <v>-50</v>
-      </c>
-      <c r="F12" s="6">
-        <v>-30</v>
+        <v>34</v>
+      </c>
+      <c r="C12" s="29">
+        <v>0</v>
+      </c>
+      <c r="D12" s="29">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="G12" s="7">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H12" s="7">
-        <v>40</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="I12" s="7">
+        <v>-20</v>
+      </c>
+      <c r="J12" s="7">
+        <v>20</v>
+      </c>
+      <c r="K12" s="7">
+        <v>-10</v>
+      </c>
+      <c r="L12" s="7">
+        <v>20</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="7">
-        <v>-70</v>
-      </c>
-      <c r="F13" s="7">
-        <v>-50</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="C13" s="29">
+        <v>0</v>
+      </c>
+      <c r="D13" s="29">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="7">
+        <v>-40</v>
+      </c>
+      <c r="H13" s="7">
+        <v>-25</v>
+      </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K13" s="7">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
+        <v>100</v>
+      </c>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="7">
+        <v>58</v>
+      </c>
+      <c r="C14" s="29">
+        <v>0</v>
+      </c>
+      <c r="D14" s="29">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="7">
         <v>-50</v>
       </c>
-      <c r="F14" s="7">
+      <c r="H14" s="7">
         <v>-30</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7">
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7">
         <v>-100</v>
       </c>
-      <c r="J14" s="7">
-        <v>0</v>
-      </c>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L14" s="7">
+        <v>0</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="7">
-        <v>30</v>
-      </c>
-      <c r="F15" s="7">
-        <v>50</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1</v>
+      </c>
+      <c r="D15" s="29">
+        <v>3</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="7">
+        <v>-50</v>
+      </c>
+      <c r="H15" s="7">
+        <v>-30</v>
+      </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K15" s="7">
+        <v>-100</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="29">
+        <v>0</v>
+      </c>
+      <c r="D16" s="29">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="7">
+        <v>-50</v>
+      </c>
+      <c r="H16" s="7">
+        <v>-30</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
+        <v>100</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="29">
+        <v>1</v>
+      </c>
+      <c r="D17" s="29">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="7">
+        <v>-50</v>
+      </c>
+      <c r="H17" s="7">
+        <v>-30</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7">
+        <v>-100</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0</v>
+      </c>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="7">
-        <v>-50</v>
-      </c>
-      <c r="F16" s="7">
-        <v>-30</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7">
-        <v>-100</v>
-      </c>
-      <c r="J16" s="7">
-        <v>0</v>
-      </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="7">
-        <v>-40</v>
-      </c>
-      <c r="F17" s="7">
-        <v>-25</v>
-      </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7">
-        <v>0</v>
-      </c>
-      <c r="J17" s="7">
-        <v>100</v>
-      </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="B20" s="7">
         <v>30</v>
@@ -1665,9 +1783,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B21" s="7">
         <v>-20</v>
@@ -1684,9 +1802,9 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B22" s="7">
         <v>60</v>
@@ -1703,9 +1821,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B23" s="7">
         <v>-10</v>
@@ -1722,9 +1840,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B24" s="7">
         <v>-10</v>
@@ -1741,9 +1859,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B25" s="7">
         <v>30</v>
@@ -1760,9 +1878,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B26" s="7">
         <v>-100</v>
@@ -1779,9 +1897,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B27" s="7">
         <v>-100</v>
@@ -1798,9 +1916,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B28" s="7">
         <v>-30</v>
@@ -1813,9 +1931,9 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B29" s="7">
         <v>-50</v>
@@ -1832,9 +1950,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B30" s="6">
         <v>-50</v>
@@ -1851,9 +1969,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B31" s="7">
         <v>60</v>
@@ -1870,7 +1988,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1879,12 +1997,12 @@
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
@@ -1902,26 +2020,26 @@
       <c r="P34" s="9"/>
       <c r="Q34" s="9"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="17" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="19" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G35" s="20"/>
       <c r="H35" s="19" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I35" s="20"/>
       <c r="J35" s="27" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K35" s="28"/>
       <c r="L35" s="10"/>
@@ -1931,37 +2049,37 @@
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="15" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="J36" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L36" s="10"/>
       <c r="M36" s="9"/>
@@ -1970,9 +2088,9 @@
       <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B37" s="16">
         <v>20</v>
@@ -2007,9 +2125,9 @@
       <c r="P37" s="9"/>
       <c r="Q37" s="9"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B38" s="7">
         <v>90</v>
@@ -2044,9 +2162,9 @@
       <c r="P38" s="9"/>
       <c r="Q38" s="9"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B39" s="7">
         <v>10</v>
@@ -2081,9 +2199,9 @@
       <c r="P39" s="9"/>
       <c r="Q39" s="9"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B40" s="7">
         <v>20</v>
@@ -2118,9 +2236,9 @@
       <c r="P40" s="9"/>
       <c r="Q40" s="9"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B41" s="7">
         <v>70</v>
@@ -2155,9 +2273,9 @@
       <c r="P41" s="9"/>
       <c r="Q41" s="9"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B42" s="7">
         <v>70</v>
@@ -2192,9 +2310,9 @@
       <c r="P42" s="9"/>
       <c r="Q42" s="9"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B43" s="7">
         <v>0</v>
@@ -2229,9 +2347,9 @@
       <c r="P43" s="9"/>
       <c r="Q43" s="9"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B44" s="7">
         <v>0</v>
@@ -2266,9 +2384,9 @@
       <c r="P44" s="9"/>
       <c r="Q44" s="9"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B45" s="7">
         <v>50</v>
@@ -2303,9 +2421,9 @@
       <c r="P45" s="9"/>
       <c r="Q45" s="9"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B46" s="7">
         <v>30</v>
@@ -2340,9 +2458,9 @@
       <c r="P46" s="9"/>
       <c r="Q46" s="9"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B47" s="7">
         <v>30</v>
@@ -2377,9 +2495,9 @@
       <c r="P47" s="9"/>
       <c r="Q47" s="9"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B48" s="7">
         <v>80</v>
@@ -2414,7 +2532,7 @@
       <c r="P48" s="9"/>
       <c r="Q48" s="9"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -2433,74 +2551,74 @@
       <c r="P50" s="9"/>
       <c r="Q50" s="9"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
-    <sortCondition ref="A2:A17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S17">
+    <sortCondition ref="B2:B17"/>
   </sortState>
   <mergeCells count="7">
     <mergeCell ref="B35:C35"/>
@@ -2511,7 +2629,7 @@
     <mergeCell ref="B34:K34"/>
     <mergeCell ref="J35:K35"/>
   </mergeCells>
-  <conditionalFormatting sqref="A34 A50 A53:A64 A37:A48 A20:A32 C2:D17">
+  <conditionalFormatting sqref="A34 A50 A53:A64 A37:A48 A20:A32 E2:F17">
     <cfRule type="cellIs" dxfId="38" priority="127" operator="equal">
       <formula>$A$55</formula>
     </cfRule>
@@ -2533,7 +2651,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A34 A50 C2:D17 A53:A70</xm:sqref>
+          <xm:sqref>A34 A50 E2:F17 A53:A70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="96" operator="containsText" id="{BFB7F44B-5851-4A42-BEFF-EEAC6C535F2D}">
@@ -2596,7 +2714,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="59" operator="containsText" id="{9CA99472-1E6A-4A77-8283-C654522B2A3D}">
-            <xm:f>NOT(ISERROR(SEARCH($A$61,C2)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($A$61,E2)))</xm:f>
             <xm:f>$A$61</xm:f>
             <x14:dxf>
               <fill>
@@ -2606,11 +2724,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C2:D2</xm:sqref>
+          <xm:sqref>E2:F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="50" operator="containsText" id="{9F6F0A46-2A4F-431E-9291-4A0F518B2144}">
-            <xm:f>NOT(ISERROR(SEARCH($A$61,C3)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($A$61,E3)))</xm:f>
             <xm:f>$A$61</xm:f>
             <x14:dxf>
               <fill>
@@ -2620,11 +2738,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C3:D13</xm:sqref>
+          <xm:sqref>E3:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="49" operator="containsText" id="{22B2448C-8DC5-4BBD-9C79-170050EAEF75}">
-            <xm:f>NOT(ISERROR(SEARCH($A$58,C6)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($A$58,E6)))</xm:f>
             <xm:f>$A$58</xm:f>
             <x14:dxf>
               <fill>
@@ -2634,7 +2752,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C6:D6</xm:sqref>
+          <xm:sqref>E6:F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="31" operator="containsText" id="{320B501C-F7DD-439D-80FA-6E914366AB96}">
@@ -2766,7 +2884,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A34 A50 A53:A64 A37:A48 A20:A32 C2:D17</xm:sqref>
+          <xm:sqref>A34 A50 A53:A64 A37:A48 A20:A32 E2:F17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="20" operator="containsText" id="{B151DFDC-3A56-4664-8AF1-A08747569E11}">
@@ -3043,7 +3161,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{B010002F-62A8-481D-9624-6449378892BB}">
-            <xm:f>NOT(ISERROR(SEARCH($A$58,C2)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($A$58,E2)))</xm:f>
             <xm:f>$A$58</xm:f>
             <x14:dxf>
               <font>
@@ -3056,11 +3174,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C2:D17</xm:sqref>
+          <xm:sqref>E2:F17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="1" operator="containsText" id="{FC1D78D0-D9CA-41EE-A99E-BA8E0CD92556}">
-            <xm:f>NOT(ISERROR(SEARCH($A$57,C2)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($A$57,E2)))</xm:f>
             <xm:f>$A$57</xm:f>
             <x14:dxf>
               <fill>
@@ -3070,7 +3188,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C2:D17</xm:sqref>
+          <xm:sqref>E2:F17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>